<commit_message>
Done with exercie 2.1
</commit_message>
<xml_diff>
--- a/Chapter 2/mortality_wide.xlsx
+++ b/Chapter 2/mortality_wide.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>1-4 Years</t>
+    <t>01-04 Years</t>
+  </si>
+  <si>
+    <t>05-09 Years</t>
   </si>
   <si>
     <t>10-14 Years</t>
   </si>
   <si>
     <t>15-19 Years</t>
-  </si>
-  <si>
-    <t>5-9 Years</t>
   </si>
   <si>
     <t>Year</t>
@@ -417,13 +417,13 @@
         <v>0.019838</v>
       </c>
       <c r="C2">
+        <v>0.004661</v>
+      </c>
+      <c r="D2">
         <v>0.002983</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.004848</v>
-      </c>
-      <c r="E2">
-        <v>0.004661</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -434,13 +434,13 @@
         <v>0.01695</v>
       </c>
       <c r="C3">
+        <v>0.004276</v>
+      </c>
+      <c r="D3">
         <v>0.002736</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.004543999999999999</v>
-      </c>
-      <c r="E3">
-        <v>0.004276</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -451,13 +451,13 @@
         <v>0.016557</v>
       </c>
       <c r="C4">
+        <v>0.004033</v>
+      </c>
+      <c r="D4">
         <v>0.002525</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.004215</v>
-      </c>
-      <c r="E4">
-        <v>0.004033</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -468,13 +468,13 @@
         <v>0.015421</v>
       </c>
       <c r="C5">
+        <v>0.004147</v>
+      </c>
+      <c r="D5">
         <v>0.002682</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.004341</v>
-      </c>
-      <c r="E5">
-        <v>0.004147</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -485,13 +485,13 @@
         <v>0.015915</v>
       </c>
       <c r="C6">
+        <v>0.00425</v>
+      </c>
+      <c r="D6">
         <v>0.003052</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.004713999999999999</v>
-      </c>
-      <c r="E6">
-        <v>0.00425</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -502,13 +502,13 @@
         <v>0.014989</v>
       </c>
       <c r="C7">
+        <v>0.003963</v>
+      </c>
+      <c r="D7">
         <v>0.002798</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.004393</v>
-      </c>
-      <c r="E7">
-        <v>0.003963</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -519,13 +519,13 @@
         <v>0.0158</v>
       </c>
       <c r="C8">
+        <v>0.003774</v>
+      </c>
+      <c r="D8">
         <v>0.002722</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.004452</v>
-      </c>
-      <c r="E8">
-        <v>0.003774</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -536,13 +536,13 @@
         <v>0.014683</v>
       </c>
       <c r="C9">
+        <v>0.003656</v>
+      </c>
+      <c r="D9">
         <v>0.002658</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.004377</v>
-      </c>
-      <c r="E9">
-        <v>0.003656</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -553,13 +553,13 @@
         <v>0.013968</v>
       </c>
       <c r="C10">
+        <v>0.003542</v>
+      </c>
+      <c r="D10">
         <v>0.002479</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0.003977</v>
-      </c>
-      <c r="E10">
-        <v>0.003542</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -570,13 +570,13 @@
         <v>0.013489</v>
       </c>
       <c r="C11">
+        <v>0.003302</v>
+      </c>
+      <c r="D11">
         <v>0.002305</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0.003636</v>
-      </c>
-      <c r="E11">
-        <v>0.003302</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -587,13 +587,13 @@
         <v>0.013973</v>
       </c>
       <c r="C12">
+        <v>0.003484</v>
+      </c>
+      <c r="D12">
         <v>0.002359</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0.003719</v>
-      </c>
-      <c r="E12">
-        <v>0.003484</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -604,13 +604,13 @@
         <v>0.01176</v>
       </c>
       <c r="C13">
+        <v>0.0031</v>
+      </c>
+      <c r="D13">
         <v>0.002222</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>0.00366</v>
-      </c>
-      <c r="E13">
-        <v>0.0031</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -621,13 +621,13 @@
         <v>0.010941</v>
       </c>
       <c r="C14">
+        <v>0.002875</v>
+      </c>
+      <c r="D14">
         <v>0.002022</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>0.003472</v>
-      </c>
-      <c r="E14">
-        <v>0.002875</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -638,13 +638,13 @@
         <v>0.011934</v>
       </c>
       <c r="C15">
+        <v>0.003177</v>
+      </c>
+      <c r="D15">
         <v>0.002148</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>0.003603</v>
-      </c>
-      <c r="E15">
-        <v>0.003177</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -655,13 +655,13 @@
         <v>0.010242</v>
       </c>
       <c r="C16">
+        <v>0.002916</v>
+      </c>
+      <c r="D16">
         <v>0.002072</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>0.003405</v>
-      </c>
-      <c r="E16">
-        <v>0.002916</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -672,13 +672,13 @@
         <v>0.009242</v>
       </c>
       <c r="C17">
+        <v>0.002606</v>
+      </c>
+      <c r="D17">
         <v>0.001967</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>0.003309</v>
-      </c>
-      <c r="E17">
-        <v>0.002606</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -689,13 +689,13 @@
         <v>0.011115</v>
       </c>
       <c r="C18">
+        <v>0.002824</v>
+      </c>
+      <c r="D18">
         <v>0.002051</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>0.003558</v>
-      </c>
-      <c r="E18">
-        <v>0.002824</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -706,13 +706,13 @@
         <v>0.01066</v>
       </c>
       <c r="C19">
+        <v>0.002907</v>
+      </c>
+      <c r="D19">
         <v>0.002189</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>0.003803</v>
-      </c>
-      <c r="E19">
-        <v>0.002907</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -723,13 +723,13 @@
         <v>0.015735</v>
       </c>
       <c r="C20">
+        <v>0.004478999999999999</v>
+      </c>
+      <c r="D20">
         <v>0.003751</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>0.007774</v>
-      </c>
-      <c r="E20">
-        <v>0.004478999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -740,13 +740,13 @@
         <v>0.00928</v>
       </c>
       <c r="C21">
+        <v>0.003</v>
+      </c>
+      <c r="D21">
         <v>0.002364</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>0.004385</v>
-      </c>
-      <c r="E21">
-        <v>0.003</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -757,13 +757,13 @@
         <v>0.009872000000000001</v>
       </c>
       <c r="C22">
+        <v>0.002952</v>
+      </c>
+      <c r="D22">
         <v>0.002299</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>0.004029</v>
-      </c>
-      <c r="E22">
-        <v>0.002952</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -774,13 +774,13 @@
         <v>0.008012</v>
       </c>
       <c r="C23">
+        <v>0.002814</v>
+      </c>
+      <c r="D23">
         <v>0.002099</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>0.003265</v>
-      </c>
-      <c r="E23">
-        <v>0.002814</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -791,13 +791,13 @@
         <v>0.00742</v>
       </c>
       <c r="C24">
+        <v>0.002396</v>
+      </c>
+      <c r="D24">
         <v>0.001866</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>0.003196</v>
-      </c>
-      <c r="E24">
-        <v>0.002396</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -808,13 +808,13 @@
         <v>0.008067000000000001</v>
       </c>
       <c r="C25">
+        <v>0.0024</v>
+      </c>
+      <c r="D25">
         <v>0.001882</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>0.003258</v>
-      </c>
-      <c r="E25">
-        <v>0.0024</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -825,13 +825,13 @@
         <v>0.006832</v>
       </c>
       <c r="C26">
+        <v>0.002217</v>
+      </c>
+      <c r="D26">
         <v>0.001798</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>0.003135</v>
-      </c>
-      <c r="E26">
-        <v>0.002217</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -842,13 +842,13 @@
         <v>0.00641</v>
       </c>
       <c r="C27">
+        <v>0.002115</v>
+      </c>
+      <c r="D27">
         <v>0.00181</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>0.00314</v>
-      </c>
-      <c r="E27">
-        <v>0.002115</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -859,13 +859,13 @@
         <v>0.007234</v>
       </c>
       <c r="C28">
+        <v>0.002138</v>
+      </c>
+      <c r="D28">
         <v>0.001714</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>0.003075</v>
-      </c>
-      <c r="E28">
-        <v>0.002138</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -876,13 +876,13 @@
         <v>0.00591</v>
       </c>
       <c r="C29">
+        <v>0.002083</v>
+      </c>
+      <c r="D29">
         <v>0.001675</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>0.002895</v>
-      </c>
-      <c r="E29">
-        <v>0.002083</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -893,13 +893,13 @@
         <v>0.006475</v>
       </c>
       <c r="C30">
+        <v>0.002131</v>
+      </c>
+      <c r="D30">
         <v>0.001738</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>0.003078</v>
-      </c>
-      <c r="E30">
-        <v>0.002131</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -910,13 +910,13 @@
         <v>0.006255</v>
       </c>
       <c r="C31">
+        <v>0.00208</v>
+      </c>
+      <c r="D31">
         <v>0.00165</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>0.00298</v>
-      </c>
-      <c r="E31">
-        <v>0.00208</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -927,13 +927,13 @@
         <v>0.005636</v>
       </c>
       <c r="C32">
+        <v>0.001898</v>
+      </c>
+      <c r="D32">
         <v>0.001528</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>0.002778</v>
-      </c>
-      <c r="E32">
-        <v>0.001898</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -944,13 +944,13 @@
         <v>0.005266</v>
       </c>
       <c r="C33">
+        <v>0.00182</v>
+      </c>
+      <c r="D33">
         <v>0.001503</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>0.002635</v>
-      </c>
-      <c r="E33">
-        <v>0.00182</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -961,13 +961,13 @@
         <v>0.004619</v>
       </c>
       <c r="C34">
+        <v>0.001659</v>
+      </c>
+      <c r="D34">
         <v>0.001422</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>0.002375</v>
-      </c>
-      <c r="E34">
-        <v>0.001659</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -978,13 +978,13 @@
         <v>0.004726</v>
       </c>
       <c r="C35">
+        <v>0.001613</v>
+      </c>
+      <c r="D35">
         <v>0.00138</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>0.002234</v>
-      </c>
-      <c r="E35">
-        <v>0.001613</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -995,13 +995,13 @@
         <v>0.005077</v>
       </c>
       <c r="C36">
+        <v>0.001651</v>
+      </c>
+      <c r="D36">
         <v>0.001415</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>0.00224</v>
-      </c>
-      <c r="E36">
-        <v>0.001651</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1012,13 +1012,13 @@
         <v>0.004409</v>
       </c>
       <c r="C37">
+        <v>0.001624</v>
+      </c>
+      <c r="D37">
         <v>0.001434</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>0.002223</v>
-      </c>
-      <c r="E37">
-        <v>0.001624</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1029,13 +1029,13 @@
         <v>0.004398</v>
       </c>
       <c r="C38">
+        <v>0.001546</v>
+      </c>
+      <c r="D38">
         <v>0.00141</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>0.002304</v>
-      </c>
-      <c r="E38">
-        <v>0.001546</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1046,13 +1046,13 @@
         <v>0.004187</v>
       </c>
       <c r="C39">
+        <v>0.001429</v>
+      </c>
+      <c r="D39">
         <v>0.001283</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>0.00219</v>
-      </c>
-      <c r="E39">
-        <v>0.001429</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1063,13 +1063,13 @@
         <v>0.003838</v>
       </c>
       <c r="C40">
+        <v>0.001288</v>
+      </c>
+      <c r="D40">
         <v>0.001138</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>0.001923</v>
-      </c>
-      <c r="E40">
-        <v>0.001288</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1080,13 +1080,13 @@
         <v>0.003183</v>
       </c>
       <c r="C41">
+        <v>0.001126</v>
+      </c>
+      <c r="D41">
         <v>0.001065</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>0.001798</v>
-      </c>
-      <c r="E41">
-        <v>0.001126</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1097,13 +1097,13 @@
         <v>0.002896</v>
       </c>
       <c r="C42">
+        <v>0.001083</v>
+      </c>
+      <c r="D42">
         <v>0.000995</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>0.001716</v>
-      </c>
-      <c r="E42">
-        <v>0.001083</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1114,13 +1114,13 @@
         <v>0.002799</v>
       </c>
       <c r="C43">
+        <v>0.001038</v>
+      </c>
+      <c r="D43">
         <v>0.000947</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>0.00169</v>
-      </c>
-      <c r="E43">
-        <v>0.001038</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1131,13 +1131,13 @@
         <v>0.002434</v>
       </c>
       <c r="C44">
+        <v>0.0009609999999999999</v>
+      </c>
+      <c r="D44">
         <v>0.0008579999999999999</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>0.001547</v>
-      </c>
-      <c r="E44">
-        <v>0.0009609999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1148,13 +1148,13 @@
         <v>0.002564</v>
       </c>
       <c r="C45">
+        <v>0.001031</v>
+      </c>
+      <c r="D45">
         <v>0.0009059999999999999</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>0.00164</v>
-      </c>
-      <c r="E45">
-        <v>0.001031</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1165,13 +1165,13 @@
         <v>0.00233</v>
       </c>
       <c r="C46">
+        <v>0.000987</v>
+      </c>
+      <c r="D46">
         <v>0.000897</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>0.001579</v>
-      </c>
-      <c r="E46">
-        <v>0.000987</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1182,13 +1182,13 @@
         <v>0.00203</v>
       </c>
       <c r="C47">
+        <v>0.000936</v>
+      </c>
+      <c r="D47">
         <v>0.000868</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>0.001523</v>
-      </c>
-      <c r="E47">
-        <v>0.000936</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1199,13 +1199,13 @@
         <v>0.001815</v>
       </c>
       <c r="C48">
+        <v>0.000856</v>
+      </c>
+      <c r="D48">
         <v>0.0007859999999999999</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>0.001378</v>
-      </c>
-      <c r="E48">
-        <v>0.000856</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1216,13 +1216,13 @@
         <v>0.001608</v>
       </c>
       <c r="C49">
+        <v>0.0007329999999999999</v>
+      </c>
+      <c r="D49">
         <v>0.000679</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>0.001268</v>
-      </c>
-      <c r="E49">
-        <v>0.0007329999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1233,13 +1233,13 @@
         <v>0.001601</v>
       </c>
       <c r="C50">
+        <v>0.0007059999999999999</v>
+      </c>
+      <c r="D50">
         <v>0.0006559999999999999</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>0.001187</v>
-      </c>
-      <c r="E50">
-        <v>0.0007059999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1250,13 +1250,13 @@
         <v>0.001502</v>
       </c>
       <c r="C51">
+        <v>0.000682</v>
+      </c>
+      <c r="D51">
         <v>0.0006360000000000001</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>0.001118</v>
-      </c>
-      <c r="E51">
-        <v>0.000682</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1267,13 +1267,13 @@
         <v>0.001394</v>
       </c>
       <c r="C52">
+        <v>0.000617</v>
+      </c>
+      <c r="D52">
         <v>0.000581</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>0.001086</v>
-      </c>
-      <c r="E52">
-        <v>0.000617</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1284,13 +1284,13 @@
         <v>0.001369</v>
       </c>
       <c r="C53">
+        <v>0.000617</v>
+      </c>
+      <c r="D53">
         <v>0.0005639999999999999</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>0.001089</v>
-      </c>
-      <c r="E53">
-        <v>0.000617</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1301,13 +1301,13 @@
         <v>0.001411</v>
       </c>
       <c r="C54">
+        <v>0.0006129999999999999</v>
+      </c>
+      <c r="D54">
         <v>0.0005679999999999999</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>0.001144</v>
-      </c>
-      <c r="E54">
-        <v>0.0006129999999999999</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1318,13 +1318,13 @@
         <v>0.0013</v>
       </c>
       <c r="C55">
+        <v>0.000561</v>
+      </c>
+      <c r="D55">
         <v>0.000531</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>0.001069</v>
-      </c>
-      <c r="E55">
-        <v>0.000561</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1335,13 +1335,13 @@
         <v>0.001183</v>
       </c>
       <c r="C56">
+        <v>0.000525</v>
+      </c>
+      <c r="D56">
         <v>0.000478</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>0.0009609999999999999</v>
-      </c>
-      <c r="E56">
-        <v>0.000525</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1352,13 +1352,13 @@
         <v>0.001134</v>
       </c>
       <c r="C57">
+        <v>0.000506</v>
+      </c>
+      <c r="D57">
         <v>0.000466</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>0.000973</v>
-      </c>
-      <c r="E57">
-        <v>0.000506</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1369,13 +1369,13 @@
         <v>0.001102</v>
       </c>
       <c r="C58">
+        <v>0.000483</v>
+      </c>
+      <c r="D58">
         <v>0.000463</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <v>0.000972</v>
-      </c>
-      <c r="E58">
-        <v>0.000483</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1386,13 +1386,13 @@
         <v>0.001118</v>
       </c>
       <c r="C59">
+        <v>0.000501</v>
+      </c>
+      <c r="D59">
         <v>0.000474</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>0.001002</v>
-      </c>
-      <c r="E59">
-        <v>0.000501</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1403,13 +1403,13 @@
         <v>0.001117</v>
       </c>
       <c r="C60">
+        <v>0.000484</v>
+      </c>
+      <c r="D60">
         <v>0.000446</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>0.000915</v>
-      </c>
-      <c r="E60">
-        <v>0.000484</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1420,13 +1420,13 @@
         <v>0.001069</v>
       </c>
       <c r="C61">
+        <v>0.000494</v>
+      </c>
+      <c r="D61">
         <v>0.000458</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>0.000928</v>
-      </c>
-      <c r="E61">
-        <v>0.000494</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1437,13 +1437,13 @@
         <v>0.001091</v>
       </c>
       <c r="C62">
+        <v>0.00049</v>
+      </c>
+      <c r="D62">
         <v>0.00044</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <v>0.0009220000000000001</v>
-      </c>
-      <c r="E62">
-        <v>0.00049</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1454,13 +1454,13 @@
         <v>0.001017</v>
       </c>
       <c r="C63">
+        <v>0.000458</v>
+      </c>
+      <c r="D63">
         <v>0.000419</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>0.0008809999999999999</v>
-      </c>
-      <c r="E63">
-        <v>0.000458</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1471,13 +1471,13 @@
         <v>0.000992</v>
       </c>
       <c r="C64">
+        <v>0.000456</v>
+      </c>
+      <c r="D64">
         <v>0.000419</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>0.0008759999999999999</v>
-      </c>
-      <c r="E64">
-        <v>0.000456</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1488,13 +1488,13 @@
         <v>0.001015</v>
       </c>
       <c r="C65">
+        <v>0.000453</v>
+      </c>
+      <c r="D65">
         <v>0.000412</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>0.000905</v>
-      </c>
-      <c r="E65">
-        <v>0.000453</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1505,13 +1505,13 @@
         <v>0.000985</v>
       </c>
       <c r="C66">
+        <v>0.000446</v>
+      </c>
+      <c r="D66">
         <v>0.000416</v>
       </c>
-      <c r="D66">
+      <c r="E66">
         <v>0.0009390000000000001</v>
-      </c>
-      <c r="E66">
-        <v>0.000446</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1522,13 +1522,13 @@
         <v>0.0009590000000000001</v>
       </c>
       <c r="C67">
+        <v>0.000439</v>
+      </c>
+      <c r="D67">
         <v>0.000405</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <v>0.000953</v>
-      </c>
-      <c r="E67">
-        <v>0.000439</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1539,13 +1539,13 @@
         <v>0.000964</v>
       </c>
       <c r="C68">
+        <v>0.000443</v>
+      </c>
+      <c r="D68">
         <v>0.000411</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>0.00102</v>
-      </c>
-      <c r="E68">
-        <v>0.000443</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1556,13 +1556,13 @@
         <v>0.000894</v>
       </c>
       <c r="C69">
+        <v>0.000429</v>
+      </c>
+      <c r="D69">
         <v>0.000405</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>0.001021</v>
-      </c>
-      <c r="E69">
-        <v>0.000429</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1573,13 +1573,13 @@
         <v>0.000896</v>
       </c>
       <c r="C70">
+        <v>0.000445</v>
+      </c>
+      <c r="D70">
         <v>0.000416</v>
       </c>
-      <c r="D70">
+      <c r="E70">
         <v>0.001081</v>
-      </c>
-      <c r="E70">
-        <v>0.000445</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1590,13 +1590,13 @@
         <v>0.00088</v>
       </c>
       <c r="C71">
+        <v>0.00044</v>
+      </c>
+      <c r="D71">
         <v>0.000413</v>
       </c>
-      <c r="D71">
+      <c r="E71">
         <v>0.001135</v>
-      </c>
-      <c r="E71">
-        <v>0.00044</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1607,13 +1607,13 @@
         <v>0.000845</v>
       </c>
       <c r="C72">
+        <v>0.000421</v>
+      </c>
+      <c r="D72">
         <v>0.000406</v>
       </c>
-      <c r="D72">
+      <c r="E72">
         <v>0.001103</v>
-      </c>
-      <c r="E72">
-        <v>0.000421</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1624,13 +1624,13 @@
         <v>0.0008229999999999999</v>
       </c>
       <c r="C73">
+        <v>0.00042</v>
+      </c>
+      <c r="D73">
         <v>0.000399</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <v>0.001103</v>
-      </c>
-      <c r="E73">
-        <v>0.00042</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1641,13 +1641,13 @@
         <v>0.000804</v>
       </c>
       <c r="C74">
+        <v>0.000408</v>
+      </c>
+      <c r="D74">
         <v>0.000404</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <v>0.001104</v>
-      </c>
-      <c r="E74">
-        <v>0.000408</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1658,13 +1658,13 @@
         <v>0.00079</v>
       </c>
       <c r="C75">
+        <v>0.000411</v>
+      </c>
+      <c r="D75">
         <v>0.000403</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <v>0.00111</v>
-      </c>
-      <c r="E75">
-        <v>0.000411</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1675,13 +1675,13 @@
         <v>0.0007329999999999999</v>
       </c>
       <c r="C76">
+        <v>0.000372</v>
+      </c>
+      <c r="D76">
         <v>0.000383</v>
       </c>
-      <c r="D76">
+      <c r="E76">
         <v>0.001048</v>
-      </c>
-      <c r="E76">
-        <v>0.000372</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1692,13 +1692,13 @@
         <v>0.0006990000000000001</v>
       </c>
       <c r="C77">
+        <v>0.000352</v>
+      </c>
+      <c r="D77">
         <v>0.000353</v>
       </c>
-      <c r="D77">
+      <c r="E77">
         <v>0.001002</v>
-      </c>
-      <c r="E77">
-        <v>0.000352</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1709,13 +1709,13 @@
         <v>0.0006879999999999999</v>
       </c>
       <c r="C78">
+        <v>0.000341</v>
+      </c>
+      <c r="D78">
         <v>0.000342</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <v>0.0009570000000000001</v>
-      </c>
-      <c r="E78">
-        <v>0.000341</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1726,13 +1726,13 @@
         <v>0.000676</v>
       </c>
       <c r="C79">
+        <v>0.000333</v>
+      </c>
+      <c r="D79">
         <v>0.000346</v>
       </c>
-      <c r="D79">
+      <c r="E79">
         <v>0.000998</v>
-      </c>
-      <c r="E79">
-        <v>0.000333</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1743,13 +1743,13 @@
         <v>0.000679</v>
       </c>
       <c r="C80">
+        <v>0.000327</v>
+      </c>
+      <c r="D80">
         <v>0.000337</v>
       </c>
-      <c r="D80">
+      <c r="E80">
         <v>0.0009890000000000001</v>
-      </c>
-      <c r="E80">
-        <v>0.000327</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1760,13 +1760,13 @@
         <v>0.000642</v>
       </c>
       <c r="C81">
+        <v>0.000311</v>
+      </c>
+      <c r="D81">
         <v>0.000318</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <v>0.0009879999999999999</v>
-      </c>
-      <c r="E81">
-        <v>0.000311</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1777,13 +1777,13 @@
         <v>0.000639</v>
       </c>
       <c r="C82">
+        <v>0.000304</v>
+      </c>
+      <c r="D82">
         <v>0.000308</v>
       </c>
-      <c r="D82">
+      <c r="E82">
         <v>0.0009790000000000001</v>
-      </c>
-      <c r="E82">
-        <v>0.000304</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -1794,13 +1794,13 @@
         <v>0.000606</v>
       </c>
       <c r="C83">
+        <v>0.000291</v>
+      </c>
+      <c r="D83">
         <v>0.000295</v>
       </c>
-      <c r="D83">
+      <c r="E83">
         <v>0.0009</v>
-      </c>
-      <c r="E83">
-        <v>0.000291</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1811,13 +1811,13 @@
         <v>0.0005820000000000001</v>
       </c>
       <c r="C84">
+        <v>0.000283</v>
+      </c>
+      <c r="D84">
         <v>0.000282</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>0.000854</v>
-      </c>
-      <c r="E84">
-        <v>0.000283</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1828,13 +1828,13 @@
         <v>0.000561</v>
       </c>
       <c r="C85">
+        <v>0.000265</v>
+      </c>
+      <c r="D85">
         <v>0.000273</v>
       </c>
-      <c r="D85">
+      <c r="E85">
         <v>0.000811</v>
-      </c>
-      <c r="E85">
-        <v>0.000265</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -1845,13 +1845,13 @@
         <v>0.000522</v>
       </c>
       <c r="C86">
+        <v>0.000253</v>
+      </c>
+      <c r="D86">
         <v>0.000283</v>
       </c>
-      <c r="D86">
+      <c r="E86">
         <v>0.000804</v>
-      </c>
-      <c r="E86">
-        <v>0.000253</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -1862,13 +1862,13 @@
         <v>0.000518</v>
       </c>
       <c r="C87">
+        <v>0.00025</v>
+      </c>
+      <c r="D87">
         <v>0.00028</v>
       </c>
-      <c r="D87">
+      <c r="E87">
         <v>0.0008050000000000001</v>
-      </c>
-      <c r="E87">
-        <v>0.00025</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1879,13 +1879,13 @@
         <v>0.0005239999999999999</v>
       </c>
       <c r="C88">
+        <v>0.000239</v>
+      </c>
+      <c r="D88">
         <v>0.000286</v>
       </c>
-      <c r="D88">
+      <c r="E88">
         <v>0.000862</v>
-      </c>
-      <c r="E88">
-        <v>0.000239</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1896,13 +1896,13 @@
         <v>0.000521</v>
       </c>
       <c r="C89">
+        <v>0.000247</v>
+      </c>
+      <c r="D89">
         <v>0.000271</v>
       </c>
-      <c r="D89">
+      <c r="E89">
         <v>0.000835</v>
-      </c>
-      <c r="E89">
-        <v>0.000247</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1913,13 +1913,13 @@
         <v>0.000515</v>
       </c>
       <c r="C90">
+        <v>0.000245</v>
+      </c>
+      <c r="D90">
         <v>0.000277</v>
       </c>
-      <c r="D90">
+      <c r="E90">
         <v>0.000867</v>
-      </c>
-      <c r="E90">
-        <v>0.000245</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -1930,13 +1930,13 @@
         <v>0.000498</v>
       </c>
       <c r="C91">
+        <v>0.000241</v>
+      </c>
+      <c r="D91">
         <v>0.000274</v>
       </c>
-      <c r="D91">
+      <c r="E91">
         <v>0.0008590000000000001</v>
-      </c>
-      <c r="E91">
-        <v>0.000241</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -1947,13 +1947,13 @@
         <v>0.000468</v>
       </c>
       <c r="C92">
+        <v>0.000222</v>
+      </c>
+      <c r="D92">
         <v>0.00026</v>
       </c>
-      <c r="D92">
+      <c r="E92">
         <v>0.000879</v>
-      </c>
-      <c r="E92">
-        <v>0.000222</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -1964,13 +1964,13 @@
         <v>0.000474</v>
       </c>
       <c r="C93">
+        <v>0.000215</v>
+      </c>
+      <c r="D93">
         <v>0.000256</v>
       </c>
-      <c r="D93">
+      <c r="E93">
         <v>0.000887</v>
-      </c>
-      <c r="E93">
-        <v>0.000215</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -1981,13 +1981,13 @@
         <v>0.000435</v>
       </c>
       <c r="C94">
+        <v>0.000203</v>
+      </c>
+      <c r="D94">
         <v>0.000244</v>
       </c>
-      <c r="D94">
+      <c r="E94">
         <v>0.0008359999999999999</v>
-      </c>
-      <c r="E94">
-        <v>0.000203</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -1998,13 +1998,13 @@
         <v>0.000446</v>
       </c>
       <c r="C95">
+        <v>0.00021</v>
+      </c>
+      <c r="D95">
         <v>0.000253</v>
       </c>
-      <c r="D95">
+      <c r="E95">
         <v>0.0008579999999999999</v>
-      </c>
-      <c r="E95">
-        <v>0.00021</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2015,13 +2015,13 @@
         <v>0.000427</v>
       </c>
       <c r="C96">
+        <v>0.000197</v>
+      </c>
+      <c r="D96">
         <v>0.000248</v>
       </c>
-      <c r="D96">
+      <c r="E96">
         <v>0.000855</v>
-      </c>
-      <c r="E96">
-        <v>0.000197</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2032,13 +2032,13 @@
         <v>0.000404</v>
       </c>
       <c r="C97">
+        <v>0.000194</v>
+      </c>
+      <c r="D97">
         <v>0.000251</v>
       </c>
-      <c r="D97">
+      <c r="E97">
         <v>0.0008209999999999999</v>
-      </c>
-      <c r="E97">
-        <v>0.000194</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2049,13 +2049,13 @@
         <v>0.00038</v>
       </c>
       <c r="C98">
+        <v>0.00019</v>
+      </c>
+      <c r="D98">
         <v>0.000234</v>
       </c>
-      <c r="D98">
+      <c r="E98">
         <v>0.000775</v>
-      </c>
-      <c r="E98">
-        <v>0.00019</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2066,13 +2066,13 @@
         <v>0.000355</v>
       </c>
       <c r="C99">
+        <v>0.00018</v>
+      </c>
+      <c r="D99">
         <v>0.000225</v>
       </c>
-      <c r="D99">
+      <c r="E99">
         <v>0.0007359999999999999</v>
-      </c>
-      <c r="E99">
-        <v>0.00018</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2083,13 +2083,13 @@
         <v>0.000341</v>
       </c>
       <c r="C100">
+        <v>0.000172</v>
+      </c>
+      <c r="D100">
         <v>0.000215</v>
       </c>
-      <c r="D100">
+      <c r="E100">
         <v>0.000695</v>
-      </c>
-      <c r="E100">
-        <v>0.000172</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2100,13 +2100,13 @@
         <v>0.000342</v>
       </c>
       <c r="C101">
+        <v>0.000169</v>
+      </c>
+      <c r="D101">
         <v>0.000204</v>
       </c>
-      <c r="D101">
+      <c r="E101">
         <v>0.000686</v>
-      </c>
-      <c r="E101">
-        <v>0.000169</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2117,13 +2117,13 @@
         <v>0.000324</v>
       </c>
       <c r="C102">
+        <v>0.000158</v>
+      </c>
+      <c r="D102">
         <v>0.000203</v>
       </c>
-      <c r="D102">
+      <c r="E102">
         <v>0.0006709999999999999</v>
-      </c>
-      <c r="E102">
-        <v>0.000158</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2134,13 +2134,13 @@
         <v>0.000334</v>
       </c>
       <c r="C103">
+        <v>0.000153</v>
+      </c>
+      <c r="D103">
         <v>0.000191</v>
       </c>
-      <c r="D103">
+      <c r="E103">
         <v>0.000663</v>
-      </c>
-      <c r="E103">
-        <v>0.000153</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2151,13 +2151,13 @@
         <v>0.000314</v>
       </c>
       <c r="C104">
+        <v>0.000152</v>
+      </c>
+      <c r="D104">
         <v>0.000194</v>
       </c>
-      <c r="D104">
+      <c r="E104">
         <v>0.00067</v>
-      </c>
-      <c r="E104">
-        <v>0.000152</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2168,13 +2168,13 @@
         <v>0.000318</v>
       </c>
       <c r="C105">
+        <v>0.000148</v>
+      </c>
+      <c r="D105">
         <v>0.000189</v>
       </c>
-      <c r="D105">
+      <c r="E105">
         <v>0.0006540000000000001</v>
-      </c>
-      <c r="E105">
-        <v>0.000148</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2185,13 +2185,13 @@
         <v>0.000303</v>
       </c>
       <c r="C106">
+        <v>0.000148</v>
+      </c>
+      <c r="D106">
         <v>0.000184</v>
       </c>
-      <c r="D106">
+      <c r="E106">
         <v>0.0006490000000000001</v>
-      </c>
-      <c r="E106">
-        <v>0.000148</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2202,13 +2202,13 @@
         <v>0.000299</v>
       </c>
       <c r="C107">
+        <v>0.000146</v>
+      </c>
+      <c r="D107">
         <v>0.000177</v>
       </c>
-      <c r="D107">
+      <c r="E107">
         <v>0.000638</v>
-      </c>
-      <c r="E107">
-        <v>0.000146</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2219,13 +2219,13 @@
         <v>0.000291</v>
       </c>
       <c r="C108">
+        <v>0.00014</v>
+      </c>
+      <c r="D108">
         <v>0.000162</v>
       </c>
-      <c r="D108">
+      <c r="E108">
         <v>0.00063</v>
-      </c>
-      <c r="E108">
-        <v>0.00014</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2236,13 +2236,13 @@
         <v>0.000294</v>
       </c>
       <c r="C109">
+        <v>0.000138</v>
+      </c>
+      <c r="D109">
         <v>0.000165</v>
       </c>
-      <c r="D109">
+      <c r="E109">
         <v>0.000603</v>
-      </c>
-      <c r="E109">
-        <v>0.000138</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2253,13 +2253,13 @@
         <v>0.000293</v>
       </c>
       <c r="C110">
+        <v>0.000126</v>
+      </c>
+      <c r="D110">
         <v>0.000152</v>
       </c>
-      <c r="D110">
+      <c r="E110">
         <v>0.000559</v>
-      </c>
-      <c r="E110">
-        <v>0.000126</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2270,13 +2270,13 @@
         <v>0.000274</v>
       </c>
       <c r="C111">
+        <v>0.000125</v>
+      </c>
+      <c r="D111">
         <v>0.000151</v>
       </c>
-      <c r="D111">
+      <c r="E111">
         <v>0.000519</v>
-      </c>
-      <c r="E111">
-        <v>0.000125</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2287,13 +2287,13 @@
         <v>0.000265</v>
       </c>
       <c r="C112">
+        <v>0.000115</v>
+      </c>
+      <c r="D112">
         <v>0.000143</v>
       </c>
-      <c r="D112">
+      <c r="E112">
         <v>0.000494</v>
-      </c>
-      <c r="E112">
-        <v>0.000115</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2304,13 +2304,13 @@
         <v>0.000263</v>
       </c>
       <c r="C113">
+        <v>0.000121</v>
+      </c>
+      <c r="D113">
         <v>0.000142</v>
       </c>
-      <c r="D113">
+      <c r="E113">
         <v>0.000489</v>
-      </c>
-      <c r="E113">
-        <v>0.000121</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2321,13 +2321,13 @@
         <v>0.000263</v>
       </c>
       <c r="C114">
+        <v>0.000114</v>
+      </c>
+      <c r="D114">
         <v>0.000139</v>
       </c>
-      <c r="D114">
+      <c r="E114">
         <v>0.000472</v>
-      </c>
-      <c r="E114">
-        <v>0.000114</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2338,13 +2338,13 @@
         <v>0.000255</v>
       </c>
       <c r="C115">
+        <v>0.000118</v>
+      </c>
+      <c r="D115">
         <v>0.000141</v>
       </c>
-      <c r="D115">
+      <c r="E115">
         <v>0.000448</v>
-      </c>
-      <c r="E115">
-        <v>0.000118</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2355,13 +2355,13 @@
         <v>0.00024</v>
       </c>
       <c r="C116">
+        <v>0.000115</v>
+      </c>
+      <c r="D116">
         <v>0.00014</v>
       </c>
-      <c r="D116">
+      <c r="E116">
         <v>0.000455</v>
-      </c>
-      <c r="E116">
-        <v>0.000115</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -2372,13 +2372,13 @@
         <v>0.000249</v>
       </c>
       <c r="C117">
+        <v>0.000117</v>
+      </c>
+      <c r="D117">
         <v>0.000146</v>
       </c>
-      <c r="D117">
+      <c r="E117">
         <v>0.000483</v>
-      </c>
-      <c r="E117">
-        <v>0.000117</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -2389,13 +2389,13 @@
         <v>0.000253</v>
       </c>
       <c r="C118">
+        <v>0.000122</v>
+      </c>
+      <c r="D118">
         <v>0.000146</v>
       </c>
-      <c r="D118">
+      <c r="E118">
         <v>0.000512</v>
-      </c>
-      <c r="E118">
-        <v>0.000122</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2406,13 +2406,13 @@
         <v>0.000243</v>
       </c>
       <c r="C119">
+        <v>0.000116</v>
+      </c>
+      <c r="D119">
         <v>0.000155</v>
       </c>
-      <c r="D119">
+      <c r="E119">
         <v>0.000515</v>
-      </c>
-      <c r="E119">
-        <v>0.000116</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -2423,13 +2423,13 @@
         <v>0.00024</v>
       </c>
       <c r="C120">
+        <v>0.000115</v>
+      </c>
+      <c r="D120">
         <v>0.000149</v>
       </c>
-      <c r="D120">
+      <c r="E120">
         <v>0.000492</v>
-      </c>
-      <c r="E120">
-        <v>0.000115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>